<commit_message>
separated the fixation and ball images pt2
</commit_message>
<xml_diff>
--- a/Experiment/Orders/PAR00_RUN01.xlsx
+++ b/Experiment/Orders/PAR00_RUN01.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kmstu\Documents\GitHub\fMRI_FaceSize_ED_2024\Experiment\Orders\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{069E4E26-1DDF-4323-AF11-83FAE0DFB927}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86839724-86EE-491E-B959-FC699F604BA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,18 +57,6 @@
   </si>
   <si>
     <t>NULL_Baseline</t>
-  </si>
-  <si>
-    <t>Fixation_D64_L.png</t>
-  </si>
-  <si>
-    <t>Fixation_D64_R.png</t>
-  </si>
-  <si>
-    <t>Fixation_D51_L.png</t>
-  </si>
-  <si>
-    <t>Fixation_D51_R.png</t>
   </si>
   <si>
     <t>NULL_ITI</t>
@@ -128,12 +116,6 @@
     <t>Face01_D64_S31</t>
   </si>
   <si>
-    <t>Fixation_D80_L.png</t>
-  </si>
-  <si>
-    <t>Fixation_D80_R.png</t>
-  </si>
-  <si>
     <t>Face01_D80_S20</t>
   </si>
   <si>
@@ -174,6 +156,24 @@
   </si>
   <si>
     <t>NULL_Change</t>
+  </si>
+  <si>
+    <t>Ball_D64_R.png</t>
+  </si>
+  <si>
+    <t>Ball_D51_R.png</t>
+  </si>
+  <si>
+    <t>Ball_D80_R.png</t>
+  </si>
+  <si>
+    <t>Ball_D64_L.png</t>
+  </si>
+  <si>
+    <t>Ball_D51_L.png</t>
+  </si>
+  <si>
+    <t>Ball_D80_L.png</t>
   </si>
 </sst>
 </file>
@@ -512,7 +512,7 @@
   <dimension ref="A1:J147"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -546,16 +546,16 @@
         <v>5</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.4">
@@ -569,10 +569,10 @@
         <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="F2" t="b">
         <v>0</v>
@@ -595,16 +595,16 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C3" s="3">
         <v>20</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="F3" t="b">
         <v>0</v>
@@ -627,16 +627,16 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C4" s="3">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F4" t="b">
         <v>0</v>
@@ -659,16 +659,16 @@
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C5" s="3">
         <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="E5" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="F5" t="b">
         <v>0</v>
@@ -691,16 +691,16 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C6" s="3">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F6" t="b">
         <v>0</v>
@@ -723,16 +723,16 @@
         <v>0</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C7" s="3">
         <v>3</v>
       </c>
       <c r="D7" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="E7" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="F7" t="b">
         <v>0</v>
@@ -755,16 +755,16 @@
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C8" s="3">
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E8" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F8" t="b">
         <v>0</v>
@@ -787,16 +787,16 @@
         <v>0</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C9" s="3">
         <v>3</v>
       </c>
       <c r="D9" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="E9" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="F9" t="b">
         <v>0</v>
@@ -819,16 +819,16 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C10" s="3">
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E10" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F10" t="b">
         <v>0</v>
@@ -851,16 +851,16 @@
         <v>0</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C11" s="3">
         <v>3</v>
       </c>
       <c r="D11" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="E11" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="F11" t="b">
         <v>0</v>
@@ -883,16 +883,16 @@
         <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C12" s="3">
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E12" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F12" t="b">
         <v>0</v>
@@ -915,16 +915,16 @@
         <v>0</v>
       </c>
       <c r="B13" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C13" s="3">
         <v>3</v>
       </c>
       <c r="D13" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="E13" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="F13" t="b">
         <v>0</v>
@@ -947,16 +947,16 @@
         <v>6</v>
       </c>
       <c r="B14" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C14" s="3">
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E14" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F14" t="b">
         <v>0</v>
@@ -979,16 +979,16 @@
         <v>0</v>
       </c>
       <c r="B15" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C15" s="3">
         <v>20</v>
       </c>
       <c r="D15" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="E15" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="F15" t="b">
         <v>0</v>
@@ -1011,16 +1011,16 @@
         <v>7</v>
       </c>
       <c r="B16" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C16" s="3">
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E16" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F16" t="b">
         <v>0</v>
@@ -1043,16 +1043,16 @@
         <v>0</v>
       </c>
       <c r="B17" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C17" s="3">
         <v>3</v>
       </c>
       <c r="D17" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="E17" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="F17" t="b">
         <v>0</v>
@@ -1075,16 +1075,16 @@
         <v>8</v>
       </c>
       <c r="B18" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C18" s="3">
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E18" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F18" t="b">
         <v>0</v>
@@ -1107,16 +1107,16 @@
         <v>0</v>
       </c>
       <c r="B19" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C19" s="3">
         <v>3</v>
       </c>
       <c r="D19" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="E19" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="F19" t="b">
         <v>0</v>
@@ -1139,16 +1139,16 @@
         <v>9</v>
       </c>
       <c r="B20" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C20" s="3">
         <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E20" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F20" t="b">
         <v>0</v>
@@ -1171,16 +1171,16 @@
         <v>0</v>
       </c>
       <c r="B21" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C21" s="3">
         <v>3</v>
       </c>
       <c r="D21" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="E21" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="F21" t="b">
         <v>0</v>
@@ -1203,16 +1203,16 @@
         <v>10</v>
       </c>
       <c r="B22" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C22" s="3">
         <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E22" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F22" t="b">
         <v>0</v>
@@ -1235,16 +1235,16 @@
         <v>0</v>
       </c>
       <c r="B23" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C23" s="3">
         <v>3</v>
       </c>
       <c r="D23" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="E23" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="F23" t="b">
         <v>0</v>
@@ -1267,16 +1267,16 @@
         <v>11</v>
       </c>
       <c r="B24" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C24" s="3">
         <v>1</v>
       </c>
       <c r="D24" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E24" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F24" t="b">
         <v>0</v>
@@ -1299,16 +1299,16 @@
         <v>0</v>
       </c>
       <c r="B25" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C25" s="3">
         <v>3</v>
       </c>
       <c r="D25" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="E25" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="F25" t="b">
         <v>0</v>
@@ -1331,16 +1331,16 @@
         <v>12</v>
       </c>
       <c r="B26" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C26" s="3">
         <v>1</v>
       </c>
       <c r="D26" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E26" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F26" t="b">
         <v>0</v>
@@ -1363,16 +1363,16 @@
         <v>0</v>
       </c>
       <c r="B27" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C27" s="3">
         <v>20</v>
       </c>
       <c r="D27" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="E27" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="F27" t="b">
         <v>0</v>
@@ -1395,16 +1395,16 @@
         <v>13</v>
       </c>
       <c r="B28" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C28" s="3">
         <v>1</v>
       </c>
       <c r="D28" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="E28" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="F28" t="b">
         <v>0</v>
@@ -1427,16 +1427,16 @@
         <v>0</v>
       </c>
       <c r="B29" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C29" s="3">
         <v>3</v>
       </c>
       <c r="D29" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="E29" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="F29" t="b">
         <v>0</v>
@@ -1459,16 +1459,16 @@
         <v>14</v>
       </c>
       <c r="B30" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C30" s="3">
         <v>1</v>
       </c>
       <c r="D30" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="E30" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="F30" t="b">
         <v>0</v>
@@ -1491,16 +1491,16 @@
         <v>0</v>
       </c>
       <c r="B31" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C31" s="3">
         <v>3</v>
       </c>
       <c r="D31" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="E31" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="F31" t="b">
         <v>0</v>
@@ -1523,16 +1523,16 @@
         <v>15</v>
       </c>
       <c r="B32" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C32" s="3">
         <v>1</v>
       </c>
       <c r="D32" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="E32" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="F32" t="b">
         <v>0</v>
@@ -1555,16 +1555,16 @@
         <v>0</v>
       </c>
       <c r="B33" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C33" s="3">
         <v>3</v>
       </c>
       <c r="D33" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="E33" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="F33" t="b">
         <v>0</v>
@@ -1587,16 +1587,16 @@
         <v>16</v>
       </c>
       <c r="B34" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C34" s="3">
         <v>1</v>
       </c>
       <c r="D34" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="E34" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="F34" t="b">
         <v>0</v>
@@ -1619,16 +1619,16 @@
         <v>0</v>
       </c>
       <c r="B35" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C35" s="3">
         <v>3</v>
       </c>
       <c r="D35" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="E35" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="F35" t="b">
         <v>0</v>
@@ -1651,16 +1651,16 @@
         <v>17</v>
       </c>
       <c r="B36" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C36" s="3">
         <v>1</v>
       </c>
       <c r="D36" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="E36" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="F36" t="b">
         <v>0</v>
@@ -1683,16 +1683,16 @@
         <v>0</v>
       </c>
       <c r="B37" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C37" s="3">
         <v>3</v>
       </c>
       <c r="D37" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="E37" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="F37" t="b">
         <v>0</v>
@@ -1715,16 +1715,16 @@
         <v>18</v>
       </c>
       <c r="B38" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C38" s="3">
         <v>1</v>
       </c>
       <c r="D38" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="E38" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="F38" t="b">
         <v>0</v>
@@ -1747,16 +1747,16 @@
         <v>0</v>
       </c>
       <c r="B39" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C39" s="3">
         <v>20</v>
       </c>
       <c r="D39" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="E39" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="F39" t="b">
         <v>0</v>
@@ -1779,16 +1779,16 @@
         <v>19</v>
       </c>
       <c r="B40" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C40" s="3">
         <v>1</v>
       </c>
       <c r="D40" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E40" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F40" t="b">
         <v>0</v>
@@ -1811,16 +1811,16 @@
         <v>0</v>
       </c>
       <c r="B41" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C41" s="3">
         <v>3</v>
       </c>
       <c r="D41" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="E41" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="F41" t="b">
         <v>0</v>
@@ -1843,16 +1843,16 @@
         <v>20</v>
       </c>
       <c r="B42" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C42" s="3">
         <v>1</v>
       </c>
       <c r="D42" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E42" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F42" t="b">
         <v>0</v>
@@ -1875,16 +1875,16 @@
         <v>0</v>
       </c>
       <c r="B43" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C43" s="3">
         <v>3</v>
       </c>
       <c r="D43" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="E43" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="F43" t="b">
         <v>0</v>
@@ -1907,16 +1907,16 @@
         <v>21</v>
       </c>
       <c r="B44" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C44" s="3">
         <v>1</v>
       </c>
       <c r="D44" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E44" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F44" t="b">
         <v>0</v>
@@ -1939,16 +1939,16 @@
         <v>0</v>
       </c>
       <c r="B45" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C45" s="3">
         <v>3</v>
       </c>
       <c r="D45" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="E45" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="F45" t="b">
         <v>0</v>
@@ -1971,16 +1971,16 @@
         <v>22</v>
       </c>
       <c r="B46" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C46" s="3">
         <v>1</v>
       </c>
       <c r="D46" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E46" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F46" t="b">
         <v>0</v>
@@ -2003,16 +2003,16 @@
         <v>0</v>
       </c>
       <c r="B47" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C47" s="3">
         <v>3</v>
       </c>
       <c r="D47" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="E47" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="F47" t="b">
         <v>0</v>
@@ -2035,16 +2035,16 @@
         <v>23</v>
       </c>
       <c r="B48" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C48" s="3">
         <v>1</v>
       </c>
       <c r="D48" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E48" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F48" t="b">
         <v>0</v>
@@ -2067,16 +2067,16 @@
         <v>0</v>
       </c>
       <c r="B49" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C49" s="3">
         <v>3</v>
       </c>
       <c r="D49" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="E49" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="F49" t="b">
         <v>0</v>
@@ -2099,16 +2099,16 @@
         <v>24</v>
       </c>
       <c r="B50" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C50" s="3">
         <v>1</v>
       </c>
       <c r="D50" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E50" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F50" t="b">
         <v>0</v>
@@ -2131,16 +2131,16 @@
         <v>0</v>
       </c>
       <c r="B51" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C51" s="3">
         <v>20</v>
       </c>
       <c r="D51" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="E51" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="F51" t="b">
         <v>0</v>
@@ -2163,16 +2163,16 @@
         <v>25</v>
       </c>
       <c r="B52" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C52" s="3">
         <v>1</v>
       </c>
       <c r="D52" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E52" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F52" t="b">
         <v>0</v>
@@ -2195,16 +2195,16 @@
         <v>0</v>
       </c>
       <c r="B53" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C53" s="3">
         <v>3</v>
       </c>
       <c r="D53" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="E53" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="F53" t="b">
         <v>0</v>
@@ -2227,16 +2227,16 @@
         <v>26</v>
       </c>
       <c r="B54" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C54" s="3">
         <v>1</v>
       </c>
       <c r="D54" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E54" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F54" t="b">
         <v>0</v>
@@ -2259,16 +2259,16 @@
         <v>0</v>
       </c>
       <c r="B55" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C55" s="3">
         <v>3</v>
       </c>
       <c r="D55" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="E55" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="F55" t="b">
         <v>0</v>
@@ -2291,16 +2291,16 @@
         <v>27</v>
       </c>
       <c r="B56" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C56" s="3">
         <v>1</v>
       </c>
       <c r="D56" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E56" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F56" t="b">
         <v>0</v>
@@ -2323,16 +2323,16 @@
         <v>0</v>
       </c>
       <c r="B57" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C57" s="3">
         <v>3</v>
       </c>
       <c r="D57" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="E57" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="F57" t="b">
         <v>0</v>
@@ -2355,16 +2355,16 @@
         <v>28</v>
       </c>
       <c r="B58" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C58" s="3">
         <v>1</v>
       </c>
       <c r="D58" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E58" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F58" t="b">
         <v>0</v>
@@ -2387,16 +2387,16 @@
         <v>0</v>
       </c>
       <c r="B59" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C59" s="3">
         <v>3</v>
       </c>
       <c r="D59" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="E59" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="F59" t="b">
         <v>0</v>
@@ -2419,16 +2419,16 @@
         <v>29</v>
       </c>
       <c r="B60" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C60" s="3">
         <v>1</v>
       </c>
       <c r="D60" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E60" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F60" t="b">
         <v>0</v>
@@ -2451,16 +2451,16 @@
         <v>0</v>
       </c>
       <c r="B61" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C61" s="3">
         <v>3</v>
       </c>
       <c r="D61" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="E61" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="F61" t="b">
         <v>0</v>
@@ -2483,16 +2483,16 @@
         <v>30</v>
       </c>
       <c r="B62" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C62" s="3">
         <v>1</v>
       </c>
       <c r="D62" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E62" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F62" t="b">
         <v>0</v>
@@ -2515,16 +2515,16 @@
         <v>0</v>
       </c>
       <c r="B63" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C63" s="3">
         <v>20</v>
       </c>
       <c r="D63" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="E63" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="F63" t="b">
         <v>0</v>
@@ -2547,16 +2547,16 @@
         <v>31</v>
       </c>
       <c r="B64" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C64" s="3">
         <v>1</v>
       </c>
       <c r="D64" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="E64" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="F64" t="b">
         <v>0</v>
@@ -2579,16 +2579,16 @@
         <v>0</v>
       </c>
       <c r="B65" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C65" s="3">
         <v>3</v>
       </c>
       <c r="D65" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="E65" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="F65" t="b">
         <v>0</v>
@@ -2611,16 +2611,16 @@
         <v>32</v>
       </c>
       <c r="B66" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C66" s="3">
         <v>1</v>
       </c>
       <c r="D66" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="E66" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="F66" t="b">
         <v>0</v>
@@ -2643,16 +2643,16 @@
         <v>0</v>
       </c>
       <c r="B67" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C67" s="3">
         <v>3</v>
       </c>
       <c r="D67" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="E67" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="F67" t="b">
         <v>0</v>
@@ -2675,16 +2675,16 @@
         <v>33</v>
       </c>
       <c r="B68" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C68" s="3">
         <v>1</v>
       </c>
       <c r="D68" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="E68" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="F68" t="b">
         <v>0</v>
@@ -2707,16 +2707,16 @@
         <v>0</v>
       </c>
       <c r="B69" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C69" s="3">
         <v>3</v>
       </c>
       <c r="D69" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="E69" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="F69" t="b">
         <v>0</v>
@@ -2739,16 +2739,16 @@
         <v>34</v>
       </c>
       <c r="B70" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C70" s="3">
         <v>1</v>
       </c>
       <c r="D70" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="E70" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="F70" t="b">
         <v>0</v>
@@ -2771,16 +2771,16 @@
         <v>0</v>
       </c>
       <c r="B71" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C71" s="3">
         <v>3</v>
       </c>
       <c r="D71" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="E71" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="F71" t="b">
         <v>0</v>
@@ -2803,16 +2803,16 @@
         <v>35</v>
       </c>
       <c r="B72" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C72" s="3">
         <v>1</v>
       </c>
       <c r="D72" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="E72" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="F72" t="b">
         <v>0</v>
@@ -2835,16 +2835,16 @@
         <v>0</v>
       </c>
       <c r="B73" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C73" s="3">
         <v>3</v>
       </c>
       <c r="D73" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="E73" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="F73" t="b">
         <v>0</v>
@@ -2867,16 +2867,16 @@
         <v>36</v>
       </c>
       <c r="B74" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C74" s="3">
         <v>1</v>
       </c>
       <c r="D74" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="E74" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="F74" t="b">
         <v>0</v>
@@ -2899,16 +2899,16 @@
         <v>0</v>
       </c>
       <c r="B75" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C75" s="3">
         <v>20</v>
       </c>
       <c r="D75" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="E75" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="F75" t="b">
         <v>0</v>
@@ -2931,16 +2931,16 @@
         <v>37</v>
       </c>
       <c r="B76" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C76" s="3">
         <v>1</v>
       </c>
       <c r="D76" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E76" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F76" t="b">
         <v>0</v>
@@ -2963,16 +2963,16 @@
         <v>0</v>
       </c>
       <c r="B77" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C77" s="3">
         <v>3</v>
       </c>
       <c r="D77" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="E77" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="F77" t="b">
         <v>0</v>
@@ -2995,16 +2995,16 @@
         <v>38</v>
       </c>
       <c r="B78" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C78" s="3">
         <v>1</v>
       </c>
       <c r="D78" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E78" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F78" t="b">
         <v>0</v>
@@ -3027,16 +3027,16 @@
         <v>0</v>
       </c>
       <c r="B79" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C79" s="3">
         <v>3</v>
       </c>
       <c r="D79" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="E79" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="F79" t="b">
         <v>0</v>
@@ -3059,16 +3059,16 @@
         <v>39</v>
       </c>
       <c r="B80" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C80" s="3">
         <v>1</v>
       </c>
       <c r="D80" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E80" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F80" t="b">
         <v>0</v>
@@ -3091,16 +3091,16 @@
         <v>0</v>
       </c>
       <c r="B81" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C81" s="3">
         <v>3</v>
       </c>
       <c r="D81" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="E81" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="F81" t="b">
         <v>0</v>
@@ -3123,16 +3123,16 @@
         <v>40</v>
       </c>
       <c r="B82" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C82" s="3">
         <v>1</v>
       </c>
       <c r="D82" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E82" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F82" t="b">
         <v>0</v>
@@ -3155,16 +3155,16 @@
         <v>0</v>
       </c>
       <c r="B83" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C83" s="3">
         <v>3</v>
       </c>
       <c r="D83" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="E83" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="F83" t="b">
         <v>0</v>
@@ -3187,16 +3187,16 @@
         <v>41</v>
       </c>
       <c r="B84" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C84" s="3">
         <v>1</v>
       </c>
       <c r="D84" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E84" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F84" t="b">
         <v>0</v>
@@ -3219,16 +3219,16 @@
         <v>0</v>
       </c>
       <c r="B85" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C85" s="3">
         <v>3</v>
       </c>
       <c r="D85" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="E85" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="F85" t="b">
         <v>0</v>
@@ -3251,16 +3251,16 @@
         <v>42</v>
       </c>
       <c r="B86" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C86" s="3">
         <v>1</v>
       </c>
       <c r="D86" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E86" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F86" t="b">
         <v>0</v>
@@ -3283,16 +3283,16 @@
         <v>0</v>
       </c>
       <c r="B87" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C87" s="3">
         <v>20</v>
       </c>
       <c r="D87" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="E87" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="F87" t="b">
         <v>0</v>
@@ -3315,16 +3315,16 @@
         <v>43</v>
       </c>
       <c r="B88" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C88" s="3">
         <v>1</v>
       </c>
       <c r="D88" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E88" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F88" t="b">
         <v>0</v>
@@ -3347,16 +3347,16 @@
         <v>0</v>
       </c>
       <c r="B89" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C89" s="3">
         <v>3</v>
       </c>
       <c r="D89" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="E89" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="F89" t="b">
         <v>0</v>
@@ -3379,16 +3379,16 @@
         <v>44</v>
       </c>
       <c r="B90" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C90" s="3">
         <v>1</v>
       </c>
       <c r="D90" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E90" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F90" t="b">
         <v>0</v>
@@ -3411,16 +3411,16 @@
         <v>0</v>
       </c>
       <c r="B91" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C91" s="3">
         <v>3</v>
       </c>
       <c r="D91" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="E91" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="F91" t="b">
         <v>0</v>
@@ -3443,16 +3443,16 @@
         <v>45</v>
       </c>
       <c r="B92" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C92" s="3">
         <v>1</v>
       </c>
       <c r="D92" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E92" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F92" t="b">
         <v>0</v>
@@ -3475,16 +3475,16 @@
         <v>0</v>
       </c>
       <c r="B93" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C93" s="3">
         <v>3</v>
       </c>
       <c r="D93" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="E93" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="F93" t="b">
         <v>0</v>
@@ -3507,16 +3507,16 @@
         <v>46</v>
       </c>
       <c r="B94" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C94" s="3">
         <v>1</v>
       </c>
       <c r="D94" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E94" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F94" t="b">
         <v>0</v>
@@ -3539,16 +3539,16 @@
         <v>0</v>
       </c>
       <c r="B95" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C95" s="3">
         <v>3</v>
       </c>
       <c r="D95" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="E95" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="F95" t="b">
         <v>0</v>
@@ -3571,16 +3571,16 @@
         <v>47</v>
       </c>
       <c r="B96" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C96" s="3">
         <v>1</v>
       </c>
       <c r="D96" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E96" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F96" t="b">
         <v>0</v>
@@ -3603,16 +3603,16 @@
         <v>0</v>
       </c>
       <c r="B97" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C97" s="3">
         <v>3</v>
       </c>
       <c r="D97" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="E97" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="F97" t="b">
         <v>0</v>
@@ -3635,16 +3635,16 @@
         <v>48</v>
       </c>
       <c r="B98" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C98" s="3">
         <v>1</v>
       </c>
       <c r="D98" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E98" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F98" t="b">
         <v>0</v>
@@ -3667,16 +3667,16 @@
         <v>0</v>
       </c>
       <c r="B99" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C99" s="3">
         <v>20</v>
       </c>
       <c r="D99" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="E99" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="F99" t="b">
         <v>0</v>
@@ -3699,16 +3699,16 @@
         <v>49</v>
       </c>
       <c r="B100" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C100" s="3">
         <v>1</v>
       </c>
       <c r="D100" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="E100" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="F100" t="b">
         <v>0</v>
@@ -3731,16 +3731,16 @@
         <v>0</v>
       </c>
       <c r="B101" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C101" s="3">
         <v>3</v>
       </c>
       <c r="D101" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="E101" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="F101" t="b">
         <v>0</v>
@@ -3763,16 +3763,16 @@
         <v>50</v>
       </c>
       <c r="B102" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C102" s="3">
         <v>1</v>
       </c>
       <c r="D102" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="E102" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="F102" t="b">
         <v>0</v>
@@ -3795,16 +3795,16 @@
         <v>0</v>
       </c>
       <c r="B103" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C103" s="3">
         <v>3</v>
       </c>
       <c r="D103" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="E103" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="F103" t="b">
         <v>0</v>
@@ -3827,16 +3827,16 @@
         <v>51</v>
       </c>
       <c r="B104" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C104" s="3">
         <v>1</v>
       </c>
       <c r="D104" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="E104" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="F104" t="b">
         <v>0</v>
@@ -3859,16 +3859,16 @@
         <v>0</v>
       </c>
       <c r="B105" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C105" s="3">
         <v>3</v>
       </c>
       <c r="D105" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="E105" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="F105" t="b">
         <v>0</v>
@@ -3891,16 +3891,16 @@
         <v>52</v>
       </c>
       <c r="B106" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C106" s="3">
         <v>1</v>
       </c>
       <c r="D106" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="E106" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="F106" t="b">
         <v>0</v>
@@ -3923,16 +3923,16 @@
         <v>0</v>
       </c>
       <c r="B107" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C107" s="3">
         <v>3</v>
       </c>
       <c r="D107" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="E107" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="F107" t="b">
         <v>0</v>
@@ -3955,16 +3955,16 @@
         <v>53</v>
       </c>
       <c r="B108" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C108" s="3">
         <v>1</v>
       </c>
       <c r="D108" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="E108" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="F108" t="b">
         <v>0</v>
@@ -3987,16 +3987,16 @@
         <v>0</v>
       </c>
       <c r="B109" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C109" s="3">
         <v>3</v>
       </c>
       <c r="D109" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="E109" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="F109" t="b">
         <v>0</v>
@@ -4019,16 +4019,16 @@
         <v>54</v>
       </c>
       <c r="B110" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C110" s="3">
         <v>1</v>
       </c>
       <c r="D110" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="E110" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="F110" t="b">
         <v>0</v>
@@ -4051,16 +4051,16 @@
         <v>0</v>
       </c>
       <c r="B111" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C111" s="3">
         <v>20</v>
       </c>
       <c r="D111" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="E111" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="F111" t="b">
         <v>0</v>
@@ -4083,16 +4083,16 @@
         <v>55</v>
       </c>
       <c r="B112" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C112" s="3">
         <v>1</v>
       </c>
       <c r="D112" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E112" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F112" t="b">
         <v>0</v>
@@ -4115,16 +4115,16 @@
         <v>0</v>
       </c>
       <c r="B113" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C113" s="3">
         <v>3</v>
       </c>
       <c r="D113" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="E113" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="F113" t="b">
         <v>0</v>
@@ -4147,16 +4147,16 @@
         <v>56</v>
       </c>
       <c r="B114" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C114" s="3">
         <v>1</v>
       </c>
       <c r="D114" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E114" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F114" t="b">
         <v>0</v>
@@ -4179,16 +4179,16 @@
         <v>0</v>
       </c>
       <c r="B115" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C115" s="3">
         <v>3</v>
       </c>
       <c r="D115" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="E115" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="F115" t="b">
         <v>0</v>
@@ -4211,16 +4211,16 @@
         <v>57</v>
       </c>
       <c r="B116" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C116" s="3">
         <v>1</v>
       </c>
       <c r="D116" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E116" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F116" t="b">
         <v>0</v>
@@ -4243,16 +4243,16 @@
         <v>0</v>
       </c>
       <c r="B117" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C117" s="3">
         <v>3</v>
       </c>
       <c r="D117" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="E117" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="F117" t="b">
         <v>0</v>
@@ -4275,16 +4275,16 @@
         <v>58</v>
       </c>
       <c r="B118" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C118" s="3">
         <v>1</v>
       </c>
       <c r="D118" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E118" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F118" t="b">
         <v>0</v>
@@ -4307,16 +4307,16 @@
         <v>0</v>
       </c>
       <c r="B119" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C119" s="3">
         <v>3</v>
       </c>
       <c r="D119" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="E119" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="F119" t="b">
         <v>0</v>
@@ -4339,16 +4339,16 @@
         <v>59</v>
       </c>
       <c r="B120" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C120" s="3">
         <v>1</v>
       </c>
       <c r="D120" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E120" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F120" t="b">
         <v>0</v>
@@ -4371,16 +4371,16 @@
         <v>0</v>
       </c>
       <c r="B121" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C121" s="3">
         <v>3</v>
       </c>
       <c r="D121" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="E121" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="F121" t="b">
         <v>0</v>
@@ -4403,16 +4403,16 @@
         <v>60</v>
       </c>
       <c r="B122" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C122" s="3">
         <v>1</v>
       </c>
       <c r="D122" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E122" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F122" t="b">
         <v>0</v>
@@ -4435,16 +4435,16 @@
         <v>0</v>
       </c>
       <c r="B123" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C123" s="3">
         <v>20</v>
       </c>
       <c r="D123" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="E123" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="F123" t="b">
         <v>0</v>
@@ -4467,16 +4467,16 @@
         <v>61</v>
       </c>
       <c r="B124" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C124" s="3">
         <v>1</v>
       </c>
       <c r="D124" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E124" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F124" t="b">
         <v>0</v>
@@ -4499,16 +4499,16 @@
         <v>0</v>
       </c>
       <c r="B125" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C125" s="3">
         <v>3</v>
       </c>
       <c r="D125" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="E125" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="F125" t="b">
         <v>0</v>
@@ -4531,16 +4531,16 @@
         <v>62</v>
       </c>
       <c r="B126" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C126" s="3">
         <v>1</v>
       </c>
       <c r="D126" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E126" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F126" t="b">
         <v>0</v>
@@ -4563,16 +4563,16 @@
         <v>0</v>
       </c>
       <c r="B127" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C127" s="3">
         <v>3</v>
       </c>
       <c r="D127" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="E127" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="F127" t="b">
         <v>0</v>
@@ -4595,16 +4595,16 @@
         <v>63</v>
       </c>
       <c r="B128" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C128" s="3">
         <v>1</v>
       </c>
       <c r="D128" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E128" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F128" t="b">
         <v>0</v>
@@ -4627,16 +4627,16 @@
         <v>0</v>
       </c>
       <c r="B129" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C129" s="3">
         <v>3</v>
       </c>
       <c r="D129" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="E129" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="F129" t="b">
         <v>0</v>
@@ -4659,16 +4659,16 @@
         <v>64</v>
       </c>
       <c r="B130" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C130" s="3">
         <v>1</v>
       </c>
       <c r="D130" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E130" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F130" t="b">
         <v>0</v>
@@ -4691,16 +4691,16 @@
         <v>0</v>
       </c>
       <c r="B131" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C131" s="3">
         <v>3</v>
       </c>
       <c r="D131" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="E131" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="F131" t="b">
         <v>0</v>
@@ -4723,16 +4723,16 @@
         <v>65</v>
       </c>
       <c r="B132" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C132" s="3">
         <v>1</v>
       </c>
       <c r="D132" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E132" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F132" t="b">
         <v>0</v>
@@ -4755,16 +4755,16 @@
         <v>0</v>
       </c>
       <c r="B133" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C133" s="3">
         <v>3</v>
       </c>
       <c r="D133" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="E133" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="F133" t="b">
         <v>0</v>
@@ -4787,16 +4787,16 @@
         <v>66</v>
       </c>
       <c r="B134" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C134" s="3">
         <v>1</v>
       </c>
       <c r="D134" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E134" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F134" t="b">
         <v>0</v>
@@ -4819,16 +4819,16 @@
         <v>0</v>
       </c>
       <c r="B135" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C135" s="3">
         <v>20</v>
       </c>
       <c r="D135" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="E135" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="F135" t="b">
         <v>0</v>
@@ -4851,16 +4851,16 @@
         <v>67</v>
       </c>
       <c r="B136" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C136" s="3">
         <v>1</v>
       </c>
       <c r="D136" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="E136" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="F136" t="b">
         <v>0</v>
@@ -4883,16 +4883,16 @@
         <v>0</v>
       </c>
       <c r="B137" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C137" s="3">
         <v>3</v>
       </c>
       <c r="D137" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="E137" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="F137" t="b">
         <v>0</v>
@@ -4915,16 +4915,16 @@
         <v>68</v>
       </c>
       <c r="B138" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C138" s="3">
         <v>1</v>
       </c>
       <c r="D138" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="E138" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="F138" t="b">
         <v>0</v>
@@ -4947,16 +4947,16 @@
         <v>0</v>
       </c>
       <c r="B139" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C139" s="3">
         <v>3</v>
       </c>
       <c r="D139" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="E139" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="F139" t="b">
         <v>0</v>
@@ -4979,16 +4979,16 @@
         <v>69</v>
       </c>
       <c r="B140" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C140" s="3">
         <v>1</v>
       </c>
       <c r="D140" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="E140" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="F140" t="b">
         <v>0</v>
@@ -5011,16 +5011,16 @@
         <v>0</v>
       </c>
       <c r="B141" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C141" s="3">
         <v>3</v>
       </c>
       <c r="D141" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="E141" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="F141" t="b">
         <v>0</v>
@@ -5043,16 +5043,16 @@
         <v>70</v>
       </c>
       <c r="B142" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C142" s="3">
         <v>1</v>
       </c>
       <c r="D142" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="E142" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="F142" t="b">
         <v>0</v>
@@ -5075,16 +5075,16 @@
         <v>0</v>
       </c>
       <c r="B143" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C143" s="3">
         <v>3</v>
       </c>
       <c r="D143" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="E143" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="F143" t="b">
         <v>0</v>
@@ -5107,16 +5107,16 @@
         <v>71</v>
       </c>
       <c r="B144" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C144" s="3">
         <v>1</v>
       </c>
       <c r="D144" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="E144" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="F144" t="b">
         <v>0</v>
@@ -5139,16 +5139,16 @@
         <v>0</v>
       </c>
       <c r="B145" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C145" s="3">
         <v>3</v>
       </c>
       <c r="D145" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="E145" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="F145" t="b">
         <v>0</v>
@@ -5171,16 +5171,16 @@
         <v>72</v>
       </c>
       <c r="B146" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C146" s="3">
         <v>1</v>
       </c>
       <c r="D146" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="E146" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="F146" t="b">
         <v>0</v>
@@ -5209,10 +5209,10 @@
         <v>20</v>
       </c>
       <c r="D147" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="E147" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="F147" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
switch ball to fixation in demo order
</commit_message>
<xml_diff>
--- a/Experiment/Orders/PAR00_RUN01.xlsx
+++ b/Experiment/Orders/PAR00_RUN01.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kmstu\Documents\GitHub\fMRI_FaceSize_ED_2024\Experiment\Orders\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86839724-86EE-491E-B959-FC699F604BA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C025446-FE69-4168-9F13-71CA5AC2A1EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -158,22 +158,22 @@
     <t>NULL_Change</t>
   </si>
   <si>
-    <t>Ball_D64_R.png</t>
+    <t>Fixation_D64_L.png</t>
   </si>
   <si>
-    <t>Ball_D51_R.png</t>
+    <t>Fixation_D64_R.png</t>
   </si>
   <si>
-    <t>Ball_D80_R.png</t>
+    <t>Fixation_D51_L.png</t>
   </si>
   <si>
-    <t>Ball_D64_L.png</t>
+    <t>Fixation_D51_R.png</t>
   </si>
   <si>
-    <t>Ball_D51_L.png</t>
+    <t>Fixation_D80_L.png</t>
   </si>
   <si>
-    <t>Ball_D80_L.png</t>
+    <t>Fixation_D80_R.png</t>
   </si>
 </sst>
 </file>
@@ -512,7 +512,7 @@
   <dimension ref="A1:J147"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -569,10 +569,10 @@
         <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F2" t="b">
         <v>0</v>
@@ -601,10 +601,10 @@
         <v>20</v>
       </c>
       <c r="D3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F3" t="b">
         <v>0</v>
@@ -665,10 +665,10 @@
         <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F5" t="b">
         <v>0</v>
@@ -729,10 +729,10 @@
         <v>3</v>
       </c>
       <c r="D7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E7" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F7" t="b">
         <v>0</v>
@@ -793,10 +793,10 @@
         <v>3</v>
       </c>
       <c r="D9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E9" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F9" t="b">
         <v>0</v>
@@ -857,10 +857,10 @@
         <v>3</v>
       </c>
       <c r="D11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E11" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F11" t="b">
         <v>0</v>
@@ -921,10 +921,10 @@
         <v>3</v>
       </c>
       <c r="D13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E13" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F13" t="b">
         <v>0</v>
@@ -985,10 +985,10 @@
         <v>20</v>
       </c>
       <c r="D15" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E15" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F15" t="b">
         <v>0</v>
@@ -1049,10 +1049,10 @@
         <v>3</v>
       </c>
       <c r="D17" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E17" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F17" t="b">
         <v>0</v>
@@ -1113,10 +1113,10 @@
         <v>3</v>
       </c>
       <c r="D19" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E19" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F19" t="b">
         <v>0</v>
@@ -1177,10 +1177,10 @@
         <v>3</v>
       </c>
       <c r="D21" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E21" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F21" t="b">
         <v>0</v>
@@ -1241,10 +1241,10 @@
         <v>3</v>
       </c>
       <c r="D23" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E23" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F23" t="b">
         <v>0</v>
@@ -1305,10 +1305,10 @@
         <v>3</v>
       </c>
       <c r="D25" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E25" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F25" t="b">
         <v>0</v>
@@ -1369,10 +1369,10 @@
         <v>20</v>
       </c>
       <c r="D27" t="s">
+        <v>44</v>
+      </c>
+      <c r="E27" t="s">
         <v>45</v>
-      </c>
-      <c r="E27" t="s">
-        <v>42</v>
       </c>
       <c r="F27" t="b">
         <v>0</v>
@@ -1433,10 +1433,10 @@
         <v>3</v>
       </c>
       <c r="D29" t="s">
+        <v>44</v>
+      </c>
+      <c r="E29" t="s">
         <v>45</v>
-      </c>
-      <c r="E29" t="s">
-        <v>42</v>
       </c>
       <c r="F29" t="b">
         <v>0</v>
@@ -1497,10 +1497,10 @@
         <v>3</v>
       </c>
       <c r="D31" t="s">
+        <v>44</v>
+      </c>
+      <c r="E31" t="s">
         <v>45</v>
-      </c>
-      <c r="E31" t="s">
-        <v>42</v>
       </c>
       <c r="F31" t="b">
         <v>0</v>
@@ -1561,10 +1561,10 @@
         <v>3</v>
       </c>
       <c r="D33" t="s">
+        <v>44</v>
+      </c>
+      <c r="E33" t="s">
         <v>45</v>
-      </c>
-      <c r="E33" t="s">
-        <v>42</v>
       </c>
       <c r="F33" t="b">
         <v>0</v>
@@ -1625,10 +1625,10 @@
         <v>3</v>
       </c>
       <c r="D35" t="s">
+        <v>44</v>
+      </c>
+      <c r="E35" t="s">
         <v>45</v>
-      </c>
-      <c r="E35" t="s">
-        <v>42</v>
       </c>
       <c r="F35" t="b">
         <v>0</v>
@@ -1689,10 +1689,10 @@
         <v>3</v>
       </c>
       <c r="D37" t="s">
+        <v>44</v>
+      </c>
+      <c r="E37" t="s">
         <v>45</v>
-      </c>
-      <c r="E37" t="s">
-        <v>42</v>
       </c>
       <c r="F37" t="b">
         <v>0</v>
@@ -1753,10 +1753,10 @@
         <v>20</v>
       </c>
       <c r="D39" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E39" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F39" t="b">
         <v>0</v>
@@ -1817,10 +1817,10 @@
         <v>3</v>
       </c>
       <c r="D41" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E41" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F41" t="b">
         <v>0</v>
@@ -1881,10 +1881,10 @@
         <v>3</v>
       </c>
       <c r="D43" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E43" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F43" t="b">
         <v>0</v>
@@ -1945,10 +1945,10 @@
         <v>3</v>
       </c>
       <c r="D45" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E45" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F45" t="b">
         <v>0</v>
@@ -2009,10 +2009,10 @@
         <v>3</v>
       </c>
       <c r="D47" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E47" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F47" t="b">
         <v>0</v>
@@ -2073,10 +2073,10 @@
         <v>3</v>
       </c>
       <c r="D49" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E49" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F49" t="b">
         <v>0</v>
@@ -2137,10 +2137,10 @@
         <v>20</v>
       </c>
       <c r="D51" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E51" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F51" t="b">
         <v>0</v>
@@ -2201,10 +2201,10 @@
         <v>3</v>
       </c>
       <c r="D53" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E53" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F53" t="b">
         <v>0</v>
@@ -2265,10 +2265,10 @@
         <v>3</v>
       </c>
       <c r="D55" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E55" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F55" t="b">
         <v>0</v>
@@ -2329,10 +2329,10 @@
         <v>3</v>
       </c>
       <c r="D57" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E57" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F57" t="b">
         <v>0</v>
@@ -2393,10 +2393,10 @@
         <v>3</v>
       </c>
       <c r="D59" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E59" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F59" t="b">
         <v>0</v>
@@ -2457,10 +2457,10 @@
         <v>3</v>
       </c>
       <c r="D61" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E61" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F61" t="b">
         <v>0</v>
@@ -2521,10 +2521,10 @@
         <v>20</v>
       </c>
       <c r="D63" t="s">
+        <v>44</v>
+      </c>
+      <c r="E63" t="s">
         <v>45</v>
-      </c>
-      <c r="E63" t="s">
-        <v>42</v>
       </c>
       <c r="F63" t="b">
         <v>0</v>
@@ -2585,10 +2585,10 @@
         <v>3</v>
       </c>
       <c r="D65" t="s">
+        <v>44</v>
+      </c>
+      <c r="E65" t="s">
         <v>45</v>
-      </c>
-      <c r="E65" t="s">
-        <v>42</v>
       </c>
       <c r="F65" t="b">
         <v>0</v>
@@ -2649,10 +2649,10 @@
         <v>3</v>
       </c>
       <c r="D67" t="s">
+        <v>44</v>
+      </c>
+      <c r="E67" t="s">
         <v>45</v>
-      </c>
-      <c r="E67" t="s">
-        <v>42</v>
       </c>
       <c r="F67" t="b">
         <v>0</v>
@@ -2713,10 +2713,10 @@
         <v>3</v>
       </c>
       <c r="D69" t="s">
+        <v>44</v>
+      </c>
+      <c r="E69" t="s">
         <v>45</v>
-      </c>
-      <c r="E69" t="s">
-        <v>42</v>
       </c>
       <c r="F69" t="b">
         <v>0</v>
@@ -2777,10 +2777,10 @@
         <v>3</v>
       </c>
       <c r="D71" t="s">
+        <v>44</v>
+      </c>
+      <c r="E71" t="s">
         <v>45</v>
-      </c>
-      <c r="E71" t="s">
-        <v>42</v>
       </c>
       <c r="F71" t="b">
         <v>0</v>
@@ -2841,10 +2841,10 @@
         <v>3</v>
       </c>
       <c r="D73" t="s">
+        <v>44</v>
+      </c>
+      <c r="E73" t="s">
         <v>45</v>
-      </c>
-      <c r="E73" t="s">
-        <v>42</v>
       </c>
       <c r="F73" t="b">
         <v>0</v>
@@ -2905,10 +2905,10 @@
         <v>20</v>
       </c>
       <c r="D75" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E75" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F75" t="b">
         <v>0</v>
@@ -2969,10 +2969,10 @@
         <v>3</v>
       </c>
       <c r="D77" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E77" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F77" t="b">
         <v>0</v>
@@ -3033,10 +3033,10 @@
         <v>3</v>
       </c>
       <c r="D79" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E79" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F79" t="b">
         <v>0</v>
@@ -3097,10 +3097,10 @@
         <v>3</v>
       </c>
       <c r="D81" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E81" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F81" t="b">
         <v>0</v>
@@ -3161,10 +3161,10 @@
         <v>3</v>
       </c>
       <c r="D83" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E83" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F83" t="b">
         <v>0</v>
@@ -3225,10 +3225,10 @@
         <v>3</v>
       </c>
       <c r="D85" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E85" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F85" t="b">
         <v>0</v>
@@ -3289,10 +3289,10 @@
         <v>20</v>
       </c>
       <c r="D87" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E87" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F87" t="b">
         <v>0</v>
@@ -3353,10 +3353,10 @@
         <v>3</v>
       </c>
       <c r="D89" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E89" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F89" t="b">
         <v>0</v>
@@ -3417,10 +3417,10 @@
         <v>3</v>
       </c>
       <c r="D91" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E91" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F91" t="b">
         <v>0</v>
@@ -3481,10 +3481,10 @@
         <v>3</v>
       </c>
       <c r="D93" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E93" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F93" t="b">
         <v>0</v>
@@ -3545,10 +3545,10 @@
         <v>3</v>
       </c>
       <c r="D95" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E95" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F95" t="b">
         <v>0</v>
@@ -3609,10 +3609,10 @@
         <v>3</v>
       </c>
       <c r="D97" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E97" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F97" t="b">
         <v>0</v>
@@ -3673,10 +3673,10 @@
         <v>20</v>
       </c>
       <c r="D99" t="s">
+        <v>44</v>
+      </c>
+      <c r="E99" t="s">
         <v>45</v>
-      </c>
-      <c r="E99" t="s">
-        <v>42</v>
       </c>
       <c r="F99" t="b">
         <v>0</v>
@@ -3737,10 +3737,10 @@
         <v>3</v>
       </c>
       <c r="D101" t="s">
+        <v>44</v>
+      </c>
+      <c r="E101" t="s">
         <v>45</v>
-      </c>
-      <c r="E101" t="s">
-        <v>42</v>
       </c>
       <c r="F101" t="b">
         <v>0</v>
@@ -3801,10 +3801,10 @@
         <v>3</v>
       </c>
       <c r="D103" t="s">
+        <v>44</v>
+      </c>
+      <c r="E103" t="s">
         <v>45</v>
-      </c>
-      <c r="E103" t="s">
-        <v>42</v>
       </c>
       <c r="F103" t="b">
         <v>0</v>
@@ -3865,10 +3865,10 @@
         <v>3</v>
       </c>
       <c r="D105" t="s">
+        <v>44</v>
+      </c>
+      <c r="E105" t="s">
         <v>45</v>
-      </c>
-      <c r="E105" t="s">
-        <v>42</v>
       </c>
       <c r="F105" t="b">
         <v>0</v>
@@ -3929,10 +3929,10 @@
         <v>3</v>
       </c>
       <c r="D107" t="s">
+        <v>44</v>
+      </c>
+      <c r="E107" t="s">
         <v>45</v>
-      </c>
-      <c r="E107" t="s">
-        <v>42</v>
       </c>
       <c r="F107" t="b">
         <v>0</v>
@@ -3993,10 +3993,10 @@
         <v>3</v>
       </c>
       <c r="D109" t="s">
+        <v>44</v>
+      </c>
+      <c r="E109" t="s">
         <v>45</v>
-      </c>
-      <c r="E109" t="s">
-        <v>42</v>
       </c>
       <c r="F109" t="b">
         <v>0</v>
@@ -4057,10 +4057,10 @@
         <v>20</v>
       </c>
       <c r="D111" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E111" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F111" t="b">
         <v>0</v>
@@ -4121,10 +4121,10 @@
         <v>3</v>
       </c>
       <c r="D113" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E113" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F113" t="b">
         <v>0</v>
@@ -4185,10 +4185,10 @@
         <v>3</v>
       </c>
       <c r="D115" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E115" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F115" t="b">
         <v>0</v>
@@ -4249,10 +4249,10 @@
         <v>3</v>
       </c>
       <c r="D117" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E117" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F117" t="b">
         <v>0</v>
@@ -4313,10 +4313,10 @@
         <v>3</v>
       </c>
       <c r="D119" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E119" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F119" t="b">
         <v>0</v>
@@ -4377,10 +4377,10 @@
         <v>3</v>
       </c>
       <c r="D121" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E121" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F121" t="b">
         <v>0</v>
@@ -4441,10 +4441,10 @@
         <v>20</v>
       </c>
       <c r="D123" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E123" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F123" t="b">
         <v>0</v>
@@ -4505,10 +4505,10 @@
         <v>3</v>
       </c>
       <c r="D125" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E125" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F125" t="b">
         <v>0</v>
@@ -4569,10 +4569,10 @@
         <v>3</v>
       </c>
       <c r="D127" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E127" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F127" t="b">
         <v>0</v>
@@ -4633,10 +4633,10 @@
         <v>3</v>
       </c>
       <c r="D129" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E129" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F129" t="b">
         <v>0</v>
@@ -4697,10 +4697,10 @@
         <v>3</v>
       </c>
       <c r="D131" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E131" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F131" t="b">
         <v>0</v>
@@ -4761,10 +4761,10 @@
         <v>3</v>
       </c>
       <c r="D133" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E133" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F133" t="b">
         <v>0</v>
@@ -4825,10 +4825,10 @@
         <v>20</v>
       </c>
       <c r="D135" t="s">
+        <v>44</v>
+      </c>
+      <c r="E135" t="s">
         <v>45</v>
-      </c>
-      <c r="E135" t="s">
-        <v>42</v>
       </c>
       <c r="F135" t="b">
         <v>0</v>
@@ -4889,10 +4889,10 @@
         <v>3</v>
       </c>
       <c r="D137" t="s">
+        <v>44</v>
+      </c>
+      <c r="E137" t="s">
         <v>45</v>
-      </c>
-      <c r="E137" t="s">
-        <v>42</v>
       </c>
       <c r="F137" t="b">
         <v>0</v>
@@ -4953,10 +4953,10 @@
         <v>3</v>
       </c>
       <c r="D139" t="s">
+        <v>44</v>
+      </c>
+      <c r="E139" t="s">
         <v>45</v>
-      </c>
-      <c r="E139" t="s">
-        <v>42</v>
       </c>
       <c r="F139" t="b">
         <v>0</v>
@@ -5017,10 +5017,10 @@
         <v>3</v>
       </c>
       <c r="D141" t="s">
+        <v>44</v>
+      </c>
+      <c r="E141" t="s">
         <v>45</v>
-      </c>
-      <c r="E141" t="s">
-        <v>42</v>
       </c>
       <c r="F141" t="b">
         <v>0</v>
@@ -5081,10 +5081,10 @@
         <v>3</v>
       </c>
       <c r="D143" t="s">
+        <v>44</v>
+      </c>
+      <c r="E143" t="s">
         <v>45</v>
-      </c>
-      <c r="E143" t="s">
-        <v>42</v>
       </c>
       <c r="F143" t="b">
         <v>0</v>
@@ -5145,10 +5145,10 @@
         <v>3</v>
       </c>
       <c r="D145" t="s">
+        <v>44</v>
+      </c>
+      <c r="E145" t="s">
         <v>45</v>
-      </c>
-      <c r="E145" t="s">
-        <v>42</v>
       </c>
       <c r="F145" t="b">
         <v>0</v>
@@ -5209,10 +5209,10 @@
         <v>20</v>
       </c>
       <c r="D147" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E147" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F147" t="b">
         <v>0</v>

</xml_diff>